<commit_message>
enhnaced appointment and reschdule extraction and storage
</commit_message>
<xml_diff>
--- a/call-summaries.xlsx
+++ b/call-summaries.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,10 +491,8 @@
           <t>Priya Sharma</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>+919876543210</t>
-        </is>
+      <c r="C2" t="n">
+        <v>919876543210</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -520,6 +518,96 @@
         </is>
       </c>
       <c r="I2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>call_20250703_102913_fa3bd916</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Vanshika panjwani</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>917823844614</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2025-07-03 04:59:13 IST</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>0:01:34</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>follow_up_needed</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>23</v>
+      </c>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>call_20250703_103052_a13f7173</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2025-07-03 05:00:52 IST</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>0:00:39</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>call_incomplete</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>15</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>This call transcript records an unsuccessful attempt by an IVF clinic to connect with a potential patient.
+**1. Call Purpose and Context:**
+*   The call was initiated by Ritika from Aveya IVF – Rajouri Garden.
+*   The purpose was to follow up on a form recently submitted by the unknown recipient (or a family member) requesting "clarity regarding fertility." This indicates a pre-existing inquiry or lead.
+**2. Patient's Main Concerns:**
+*   Based on the submitted form, the patient's primary concern was a general need for "clarity on fertility" issues. No specific details about the nature of this concern (e.g., difficulty conceiving, exploring options) were discussed.
+**3. Relevant Medical History Mentioned:**
+*   None. The call did not progress to a point where any medical history could be discussed.
+**4. Current Fertility Status:**
+*   Unknown. No information regarding the patient's current fertility status was exchanged.
+**5. Any Appointment Details Discussed:**
+*   None. Due to the call's repeated disconnections, no appointment details were discussed or scheduled.
+**6. Final Outcome of the Call:**
+*   The call was unsuccessful due to persistent technical issues leading to multiple disconnections.
+*   Ritika, the clinic representative, concluded the call, inviting the recipient to contact the clinic again at their convenience.</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>